<commit_message>
excel modified for readability and useful printing area
</commit_message>
<xml_diff>
--- a/mario_picross.xlsx
+++ b/mario_picross.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$3:$S$14</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -25,7 +28,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,6 +64,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -88,7 +97,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,20 +105,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +418,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="B3" sqref="B3:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,325 +427,373 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I2" s="8"/>
-      <c r="J2" s="8">
-        <v>1</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8">
-        <v>1</v>
-      </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8">
-        <v>2</v>
-      </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I3" s="8">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9">
+        <v>2</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+      <c r="I4" s="9">
         <v>3</v>
       </c>
-      <c r="J3" s="8">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="J4" s="9">
+        <v>1</v>
+      </c>
+      <c r="K4" s="9">
         <v>3</v>
       </c>
-      <c r="L3" s="8">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>1</v>
-      </c>
-      <c r="P3" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>1</v>
-      </c>
-      <c r="R3" s="8">
-        <v>1</v>
-      </c>
-      <c r="S3" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
+      <c r="P4" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>1</v>
+      </c>
+      <c r="R4" s="9">
+        <v>1</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6">
-        <v>1</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6">
-        <v>1</v>
-      </c>
-      <c r="P5" s="6">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>2</v>
-      </c>
-      <c r="R5" s="6"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>2</v>
+      </c>
+      <c r="R5" s="10"/>
+      <c r="S5" s="4"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="H6" s="6"/>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>2</v>
-      </c>
-      <c r="K6" s="6">
-        <v>2</v>
-      </c>
-      <c r="L6" s="6">
-        <v>2</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="H6" s="1"/>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
+      <c r="L6" s="10">
+        <v>2</v>
+      </c>
+      <c r="M6" s="10">
         <v>5</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="10">
         <v>5</v>
       </c>
-      <c r="O6" s="6">
-        <v>1</v>
-      </c>
-      <c r="P6" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="6">
-        <v>2</v>
-      </c>
-      <c r="S6" s="6">
+      <c r="O6" s="10">
+        <v>1</v>
+      </c>
+      <c r="P6" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>1</v>
+      </c>
+      <c r="R6" s="10">
+        <v>2</v>
+      </c>
+      <c r="S6" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1</v>
-      </c>
-      <c r="K7" s="5">
-        <v>2</v>
-      </c>
-      <c r="L7" s="5">
-        <v>2</v>
-      </c>
-      <c r="M7" s="5">
-        <v>2</v>
-      </c>
-      <c r="N7" s="5">
-        <v>2</v>
-      </c>
-      <c r="O7" s="5">
-        <v>2</v>
-      </c>
-      <c r="P7" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>1</v>
-      </c>
-      <c r="R7" s="5">
-        <v>1</v>
-      </c>
-      <c r="S7" s="5">
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>2</v>
+      </c>
+      <c r="L7" s="11">
+        <v>2</v>
+      </c>
+      <c r="M7" s="11">
+        <v>2</v>
+      </c>
+      <c r="N7" s="11">
+        <v>2</v>
+      </c>
+      <c r="O7" s="11">
+        <v>2</v>
+      </c>
+      <c r="P7" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>1</v>
+      </c>
+      <c r="R7" s="11">
+        <v>1</v>
+      </c>
+      <c r="S7" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="H8" s="5">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
         <v>5</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="H9" s="5">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
         <v>9</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="4"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12">
         <v>3</v>
       </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="F10" s="6">
-        <v>2</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="4"/>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="10">
         <v>3</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="4"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7">
-        <v>2</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
         <v>3</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="10">
         <v>3</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12">
         <v>4</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="G13" s="6">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="10">
         <v>4</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="3"/>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="4"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="G14" s="6">
+      <c r="A14" s="2"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="10">
         <v>7</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>